<commit_message>
uploading export from Jira & Result Report in Documentation
</commit_message>
<xml_diff>
--- a/Documentation/Team4{win}-Time Schedule.xlsx
+++ b/Documentation/Team4{win}-Time Schedule.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ani\Favorites\Desktop\DOCUMENTATION - Final Project\Final Project - documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ani\IdeaProjects\REPOS\Group-4-common-repo\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7310" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7310"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="2" r:id="rId1"/>
@@ -269,9 +269,6 @@
     <t>18-Sept-28-Sept</t>
   </si>
   <si>
-    <t>10-Oct-20-Oct</t>
-  </si>
-  <si>
     <t>29-Sept-6-Oct</t>
   </si>
   <si>
@@ -433,6 +430,9 @@
   </si>
   <si>
     <t>Memmber</t>
+  </si>
+  <si>
+    <t>10-Oct-19-Oct</t>
   </si>
 </sst>
 </file>
@@ -1889,8 +1889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X1001"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1941,7 +1941,7 @@
     </row>
     <row r="2" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="20" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B2" s="21" t="s">
         <v>7</v>
@@ -1974,7 +1974,7 @@
     <row r="4" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="25"/>
       <c r="B4" s="13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C4" s="14" t="s">
         <v>9</v>
@@ -2003,7 +2003,7 @@
     </row>
     <row r="6" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="32" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B6" s="21" t="s">
         <v>11</v>
@@ -2013,7 +2013,7 @@
       </c>
       <c r="D6" s="23"/>
       <c r="E6" s="33" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
@@ -2038,7 +2038,7 @@
     <row r="7" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="45"/>
       <c r="B7" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C7" s="46" t="s">
         <v>1</v>
@@ -2047,7 +2047,7 @@
         <v>4</v>
       </c>
       <c r="E7" s="47" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
@@ -2136,7 +2136,7 @@
         <v>14</v>
       </c>
       <c r="B10" s="39" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C10" s="22" t="s">
         <v>9</v>
@@ -2145,7 +2145,7 @@
         <v>3</v>
       </c>
       <c r="E10" s="40" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
@@ -2179,7 +2179,7 @@
         <v>9</v>
       </c>
       <c r="E11" s="35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
@@ -2241,7 +2241,7 @@
         <v>7</v>
       </c>
       <c r="E13" s="42" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -2256,7 +2256,7 @@
         <v>7</v>
       </c>
       <c r="E14" s="42" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:24" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -2271,7 +2271,7 @@
         <v>11</v>
       </c>
       <c r="E15" s="44" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:24" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -2286,7 +2286,7 @@
       </c>
       <c r="D16" s="51"/>
       <c r="E16" s="52" t="s">
-        <v>80</v>
+        <v>134</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -2301,7 +2301,7 @@
       </c>
       <c r="D17" s="23"/>
       <c r="E17" s="19" t="s">
-        <v>80</v>
+        <v>134</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -5334,7 +5334,7 @@
         <v>2</v>
       </c>
       <c r="D2" s="56" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -5346,7 +5346,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="56" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -5358,7 +5358,7 @@
         <v>0</v>
       </c>
       <c r="D4" s="56" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -5372,7 +5372,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="56" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -5384,7 +5384,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="56" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -5396,7 +5396,7 @@
         <v>1</v>
       </c>
       <c r="D7" s="56" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -5408,7 +5408,7 @@
         <v>1</v>
       </c>
       <c r="D8" s="56" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -5420,7 +5420,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="56" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -5432,7 +5432,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="56" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -5444,7 +5444,7 @@
         <v>1</v>
       </c>
       <c r="D11" s="56" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -5456,7 +5456,7 @@
         <v>1</v>
       </c>
       <c r="D12" s="56" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -5468,7 +5468,7 @@
         <v>1</v>
       </c>
       <c r="D13" s="56" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -5480,7 +5480,7 @@
         <v>0</v>
       </c>
       <c r="D14" s="56" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -5492,7 +5492,7 @@
         <v>0</v>
       </c>
       <c r="D15" s="56" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -5504,7 +5504,7 @@
         <v>2</v>
       </c>
       <c r="D16" s="56" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -5516,7 +5516,7 @@
         <v>2</v>
       </c>
       <c r="D17" s="56" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -5530,7 +5530,7 @@
         <v>2</v>
       </c>
       <c r="D18" s="56" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -5542,7 +5542,7 @@
         <v>2</v>
       </c>
       <c r="D19" s="56" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -5554,7 +5554,7 @@
         <v>0</v>
       </c>
       <c r="D20" s="56" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -5566,7 +5566,7 @@
         <v>0</v>
       </c>
       <c r="D21" s="56" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -5578,7 +5578,7 @@
         <v>0</v>
       </c>
       <c r="D22" s="56" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -5590,7 +5590,7 @@
         <v>0</v>
       </c>
       <c r="D23" s="56" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -8554,7 +8554,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F943"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
@@ -8571,39 +8571,39 @@
   <sheetData>
     <row r="1" spans="1:6" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="66" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B1" s="67" t="s">
+        <v>127</v>
+      </c>
+      <c r="C1" s="66" t="s">
         <v>128</v>
-      </c>
-      <c r="C1" s="66" t="s">
-        <v>129</v>
       </c>
       <c r="D1" s="66" t="s">
         <v>5</v>
       </c>
       <c r="E1" s="66" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F1" s="66" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="68" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" s="69" t="s">
         <v>94</v>
       </c>
-      <c r="B2" s="69" t="s">
+      <c r="C2" s="70" t="s">
         <v>95</v>
-      </c>
-      <c r="C2" s="70" t="s">
-        <v>96</v>
       </c>
       <c r="D2" s="70" t="s">
         <v>0</v>
       </c>
       <c r="E2" s="89" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F2" s="71" t="s">
         <v>2</v>
@@ -8612,16 +8612,16 @@
     <row r="3" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="72"/>
       <c r="B3" s="73" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C3" s="74" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D3" s="74" t="s">
         <v>0</v>
       </c>
       <c r="E3" s="87" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F3" s="84" t="s">
         <v>2</v>
@@ -8630,16 +8630,16 @@
     <row r="4" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="72"/>
       <c r="B4" s="73" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C4" s="74" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D4" s="74" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="87" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F4" s="84" t="s">
         <v>2</v>
@@ -8648,16 +8648,16 @@
     <row r="5" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="72"/>
       <c r="B5" s="73" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C5" s="74" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D5" s="74" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="87" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F5" s="84" t="s">
         <v>2</v>
@@ -8666,16 +8666,16 @@
     <row r="6" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="72"/>
       <c r="B6" s="73" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C6" s="74" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D6" s="74" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="87" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F6" s="84" t="s">
         <v>2</v>
@@ -8684,16 +8684,16 @@
     <row r="7" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="72"/>
       <c r="B7" s="73" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C7" s="74" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D7" s="74" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="87" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F7" s="84" t="s">
         <v>2</v>
@@ -8702,16 +8702,16 @@
     <row r="8" spans="1:6" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="76"/>
       <c r="B8" s="77" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C8" s="78" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D8" s="78" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="88" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F8" s="85" t="s">
         <v>2</v>
@@ -8719,19 +8719,19 @@
     </row>
     <row r="9" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="72" t="s">
+        <v>102</v>
+      </c>
+      <c r="B9" s="82" t="s">
         <v>103</v>
       </c>
-      <c r="B9" s="82" t="s">
-        <v>104</v>
-      </c>
       <c r="C9" s="74" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D9" s="74" t="s">
         <v>1</v>
       </c>
       <c r="E9" s="92" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F9" s="93" t="s">
         <v>0</v>
@@ -8740,16 +8740,16 @@
     <row r="10" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="72"/>
       <c r="B10" s="73" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C10" s="74" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D10" s="74" t="s">
         <v>1</v>
       </c>
       <c r="E10" s="92" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F10" s="93" t="s">
         <v>0</v>
@@ -8758,16 +8758,16 @@
     <row r="11" spans="1:6" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="72"/>
       <c r="B11" s="73" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C11" s="74" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D11" s="74" t="s">
         <v>1</v>
       </c>
       <c r="E11" s="92" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F11" s="93" t="s">
         <v>0</v>
@@ -8775,19 +8775,19 @@
     </row>
     <row r="12" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="68" t="s">
+        <v>106</v>
+      </c>
+      <c r="B12" s="69" t="s">
         <v>107</v>
       </c>
-      <c r="B12" s="69" t="s">
-        <v>108</v>
-      </c>
       <c r="C12" s="70" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D12" s="70" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="89" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F12" s="86" t="s">
         <v>2</v>
@@ -8796,16 +8796,16 @@
     <row r="13" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="72"/>
       <c r="B13" s="73" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C13" s="74" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D13" s="74" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="87" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F13" s="84" t="s">
         <v>2</v>
@@ -8814,16 +8814,16 @@
     <row r="14" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="72"/>
       <c r="B14" s="73" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C14" s="74" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D14" s="74" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="87" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F14" s="84" t="s">
         <v>2</v>
@@ -8832,16 +8832,16 @@
     <row r="15" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="72"/>
       <c r="B15" s="73" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C15" s="74" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D15" s="74" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="87" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F15" s="84" t="s">
         <v>2</v>
@@ -8850,16 +8850,16 @@
     <row r="16" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="72"/>
       <c r="B16" s="73" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C16" s="74" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D16" s="74" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="87" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F16" s="84" t="s">
         <v>2</v>
@@ -8868,16 +8868,16 @@
     <row r="17" spans="1:6" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="76"/>
       <c r="B17" s="77" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C17" s="78" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D17" s="78" t="s">
         <v>0</v>
       </c>
       <c r="E17" s="88" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F17" s="85" t="s">
         <v>2</v>
@@ -8885,19 +8885,19 @@
     </row>
     <row r="18" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="72" t="s">
+        <v>113</v>
+      </c>
+      <c r="B18" s="90" t="s">
         <v>114</v>
       </c>
-      <c r="B18" s="90" t="s">
-        <v>115</v>
-      </c>
       <c r="C18" s="87" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D18" s="74" t="s">
         <v>2</v>
       </c>
       <c r="E18" s="92" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F18" s="75" t="s">
         <v>0</v>
@@ -8906,16 +8906,16 @@
     <row r="19" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="72"/>
       <c r="B19" s="91" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C19" s="87" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D19" s="74" t="s">
         <v>2</v>
       </c>
       <c r="E19" s="92" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F19" s="84" t="s">
         <v>0</v>
@@ -8924,16 +8924,16 @@
     <row r="20" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="72"/>
       <c r="B20" s="91" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C20" s="87" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D20" s="74" t="s">
         <v>2</v>
       </c>
       <c r="E20" s="92" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F20" s="84" t="s">
         <v>0</v>
@@ -8942,16 +8942,16 @@
     <row r="21" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="72"/>
       <c r="B21" s="91" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C21" s="87" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D21" s="74" t="s">
         <v>2</v>
       </c>
       <c r="E21" s="92" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F21" s="84" t="s">
         <v>0</v>
@@ -8960,16 +8960,16 @@
     <row r="22" spans="1:6" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="72"/>
       <c r="B22" s="91" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C22" s="87" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D22" s="74" t="s">
         <v>2</v>
       </c>
       <c r="E22" s="92" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F22" s="84" t="s">
         <v>0</v>
@@ -8977,19 +8977,19 @@
     </row>
     <row r="23" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="68" t="s">
+        <v>119</v>
+      </c>
+      <c r="B23" s="83" t="s">
         <v>120</v>
       </c>
-      <c r="B23" s="83" t="s">
-        <v>121</v>
-      </c>
       <c r="C23" s="70" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D23" s="70" t="s">
         <v>0</v>
       </c>
       <c r="E23" s="70" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F23" s="86" t="s">
         <v>2</v>
@@ -8998,16 +8998,16 @@
     <row r="24" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="72"/>
       <c r="B24" s="83" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C24" s="74" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D24" s="74" t="s">
         <v>0</v>
       </c>
       <c r="E24" s="87" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F24" s="84" t="s">
         <v>2</v>
@@ -9016,16 +9016,16 @@
     <row r="25" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="72"/>
       <c r="B25" s="83" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C25" s="87" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D25" s="74" t="s">
         <v>2</v>
       </c>
       <c r="E25" s="87" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F25" s="84" t="s">
         <v>2</v>
@@ -9034,16 +9034,16 @@
     <row r="26" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="72"/>
       <c r="B26" s="83" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C26" s="87" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D26" s="74" t="s">
         <v>2</v>
       </c>
       <c r="E26" s="87" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F26" s="84" t="s">
         <v>2</v>
@@ -9052,16 +9052,16 @@
     <row r="27" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="72"/>
       <c r="B27" s="83" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C27" s="74" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D27" s="74" t="s">
         <v>0</v>
       </c>
       <c r="E27" s="87" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F27" s="84" t="s">
         <v>2</v>
@@ -9070,16 +9070,16 @@
     <row r="28" spans="1:6" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="76"/>
       <c r="B28" s="83" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C28" s="78" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D28" s="78" t="s">
         <v>0</v>
       </c>
       <c r="E28" s="88" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F28" s="85" t="s">
         <v>2</v>
@@ -9087,13 +9087,13 @@
     </row>
     <row r="29" spans="1:6" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="72" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B29" s="82" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C29" s="74" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D29" s="74" t="s">
         <v>0</v>
@@ -9103,7 +9103,7 @@
     </row>
     <row r="30" spans="1:6" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="79" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B30" s="80">
         <f>COUNTA(B2:B29)</f>

</xml_diff>